<commit_message>
working version of montecarlo_simulation_class
</commit_message>
<xml_diff>
--- a/Morningstar_Asset_Stats/etf_to_asset_class_map.xlsx
+++ b/Morningstar_Asset_Stats/etf_to_asset_class_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bfraenkel/Documents/Code/Financial_Plan/Morningstar_Asset_Stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DAF02D-DC95-7D49-A93A-3F8C10373890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4400E5BD-F11D-8E44-9A87-4B28E639D6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="25280" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>ETF</t>
   </si>
@@ -130,55 +130,43 @@
     <t>VXUS</t>
   </si>
   <si>
-    <t>Non-US Bond</t>
-  </si>
-  <si>
     <t>Real Estate</t>
   </si>
   <si>
     <t>Commodities</t>
   </si>
   <si>
-    <t>Inflation-Protected Bond</t>
-  </si>
-  <si>
-    <t>Non-US Small Cap Stock</t>
-  </si>
-  <si>
-    <t>US Short-Term Bond</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> U.S. Lg Cap Growth</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U.S. Lg Cap Val</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U.S. Mid Cap Growth</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U.S. Sm Cap Growth</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U.S. Sm Cap Val</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Foreign Industrialzed Mkts Stocks</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Emerging Mkts Stks</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U.S. Investment Grade Bonds</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U.S. High Yield Bonds</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Non-U.S. Bonds</t>
+    <t>U.S. High Yield Bonds</t>
+  </si>
+  <si>
+    <t>Non-U.S. Bonds</t>
+  </si>
+  <si>
+    <t>Emerging Mkts Stks</t>
+  </si>
+  <si>
+    <t>U.S. Sm Cap Val</t>
+  </si>
+  <si>
+    <t>U.S. Sm Cap Growth</t>
+  </si>
+  <si>
+    <t>U.S. Lg Cap Growth</t>
+  </si>
+  <si>
+    <t>U.S. Lg Cap Val</t>
+  </si>
+  <si>
+    <t>U.S. Investment Grade Bonds</t>
+  </si>
+  <si>
+    <t>U.S. Mid Cap Growth</t>
+  </si>
+  <si>
+    <t>Foreign Industrialzed Mkts Stocks</t>
   </si>
 </sst>
 </file>
@@ -549,7 +537,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -570,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -578,7 +566,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -586,7 +574,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -594,7 +582,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -602,7 +590,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -610,7 +598,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -618,7 +606,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -626,10 +614,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -637,7 +625,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -645,7 +633,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -653,7 +641,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -661,7 +649,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -669,7 +657,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,7 +665,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -685,7 +673,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -693,7 +681,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -701,7 +689,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -709,7 +697,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -717,7 +705,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -725,7 +713,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -733,7 +721,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -749,7 +737,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -757,7 +745,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -765,7 +753,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -773,7 +761,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -781,7 +769,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -789,7 +777,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -797,7 +785,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -805,7 +793,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -813,7 +801,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -821,7 +809,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -829,7 +817,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
tested run_one_year in test_run_one_year
</commit_message>
<xml_diff>
--- a/Morningstar_Asset_Stats/etf_to_asset_class_map.xlsx
+++ b/Morningstar_Asset_Stats/etf_to_asset_class_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bfraenkel/Documents/Code/Financial_Plan/Morningstar_Asset_Stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4400E5BD-F11D-8E44-9A87-4B28E639D6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F82521B-0105-5648-8EC0-C7CEF8FE1D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="25280" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>ETF</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Foreign Industrialzed Mkts Stocks</t>
+  </si>
+  <si>
+    <t>PDBC</t>
   </si>
 </sst>
 </file>
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -646,39 +649,39 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
@@ -686,63 +689,63 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>46</v>
@@ -750,7 +753,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
@@ -758,73 +761,81 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>